<commit_message>
SCRUM-111 Updated WebApplication test cases
</commit_message>
<xml_diff>
--- a/Testing/TestCases-WebApplication.xlsx
+++ b/Testing/TestCases-WebApplication.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI 9 months\Project Mangement M.H\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\Car-Purchasing\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E396AD6-9CFC-4A4A-8A2A-3E8DF60B76F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Test Title</t>
   </si>
@@ -108,12 +109,18 @@
   <si>
     <t>SRS_199</t>
   </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,7 +149,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +170,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +240,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -241,118 +260,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral 2" xfId="1"/>
+    <cellStyle name="Neutral 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -366,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -406,9 +325,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -443,7 +362,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -478,7 +397,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -651,27 +570,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" customWidth="1"/>
-    <col min="5" max="5" width="32.21875" customWidth="1"/>
-    <col min="6" max="6" width="42.109375" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="31.2">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -700,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="93.6">
+    <row r="2" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -722,14 +641,14 @@
       <c r="G2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="124.8">
+    <row r="3" spans="1:9" ht="126" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -754,8 +673,8 @@
       <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
+      <c r="I3" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>